<commit_message>
metadata files demo to example
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32029DA9-461D-524F-888E-FC752D9B0FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2154175-CD04-094E-8E76-8CFB594798A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="2060" windowWidth="29460" windowHeight="14100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,17 @@
     <sheet name="Detectors" sheetId="8" r:id="rId8"/>
     <sheet name="SensingPerspective" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="187">
   <si>
     <t>Attribute</t>
   </si>
@@ -206,9 +215,6 @@
     <t>hasco:hasOperatingTemperatureUnit</t>
   </si>
   <si>
-    <t>vstoi:Questionnaire</t>
-  </si>
-  <si>
     <t>vstoi:isInstrumentAttachment</t>
   </si>
   <si>
@@ -570,13 +576,40 @@
   </si>
   <si>
     <t>Dietary Questionnaire - Dietary Recall</t>
+  </si>
+  <si>
+    <t>nhanes:00063</t>
+  </si>
+  <si>
+    <t>nhanes:00064</t>
+  </si>
+  <si>
+    <t>nhanes:00065</t>
+  </si>
+  <si>
+    <t>nhanes:00066</t>
+  </si>
+  <si>
+    <t>nhanes:00067</t>
+  </si>
+  <si>
+    <t>nhanes:00068</t>
+  </si>
+  <si>
+    <t>skos:description</t>
+  </si>
+  <si>
+    <t>owl:sameAs</t>
+  </si>
+  <si>
+    <t>point to the PDF file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -616,6 +649,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2073,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2113,19 +2151,19 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>28</v>
@@ -2133,19 +2171,19 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>28</v>
@@ -2153,19 +2191,19 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>28</v>
@@ -2173,19 +2211,19 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>28</v>
@@ -5376,7 +5414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5384,7 +5424,8 @@
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
     <col min="3" max="3" width="74.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
     <col min="27" max="1025" width="11.1640625" customWidth="1"/>
   </cols>
@@ -5402,20 +5443,28 @@
       <c r="D1" t="s">
         <v>38</v>
       </c>
+      <c r="E1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>186</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -5439,13 +5488,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
@@ -5473,24 +5522,24 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -5518,519 +5567,519 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6981,6 +7030,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -8050,7 +8100,7 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8058,10 +8108,10 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9021,34 +9071,34 @@
         <v>19</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>

</xml_diff>

<commit_message>
add owl:sameAs to questionnaire PDFs
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2154175-CD04-094E-8E76-8CFB594798A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE350561-0D83-0846-86B0-B6F9E617AFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="237">
   <si>
     <t>Attribute</t>
   </si>
@@ -596,13 +596,163 @@
     <t>nhanes:00068</t>
   </si>
   <si>
-    <t>skos:description</t>
-  </si>
-  <si>
     <t>owl:sameAs</t>
   </si>
   <si>
-    <t>point to the PDF file</t>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/CBQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DMQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/FSQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/HOQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/INQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/OCQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SMQ_Family_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/ACQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/AUQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/BPQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/CDQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DMQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DEQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DIQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DBQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DSQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DLQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/ECQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/HIQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/HEQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/HUQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/IMQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/KIQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/MCQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/OCQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/OHQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/OSQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/PAQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/PFQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SLQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SMQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/WHQ_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/ALQ_ACASI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DUQ_ACASI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SXQ_ACASI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SMQ_ACASI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/ALQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/HSQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/DPQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/KIQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/PUQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/PAQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/RHQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SXQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/SMQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/VTQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/WHQ_CAPI_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/FCBS_PFU_Handcards_J.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/FCBS-CBQ-J-508.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/DSA_I.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2017-2018/questionnaires/Dietary-Post-Recall-2017-2018-508.pdf</t>
+  </si>
+  <si>
+    <t>skos:definition</t>
   </si>
 </sst>
 </file>
@@ -687,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,6 +852,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5414,8 +5565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5423,9 +5574,9 @@
     <col min="1" max="1" width="58.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
     <col min="3" max="3" width="74.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
     <col min="27" max="1025" width="11.1640625" customWidth="1"/>
   </cols>
@@ -5444,10 +5595,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -5463,7 +5614,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5498,7 +5649,9 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>186</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -5530,6 +5683,9 @@
       <c r="C4" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -5543,7 +5699,9 @@
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -5575,6 +5733,9 @@
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
+      <c r="F6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
@@ -5586,6 +5747,9 @@
       <c r="C7" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="F7" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
@@ -5597,6 +5761,9 @@
       <c r="C8" s="9" t="s">
         <v>92</v>
       </c>
+      <c r="F8" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
@@ -5608,6 +5775,9 @@
       <c r="C9" s="9" t="s">
         <v>97</v>
       </c>
+      <c r="F9" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -5619,6 +5789,9 @@
       <c r="C10" s="9" t="s">
         <v>98</v>
       </c>
+      <c r="F10" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
@@ -5630,6 +5803,9 @@
       <c r="C11" s="9" t="s">
         <v>99</v>
       </c>
+      <c r="F11" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -5641,6 +5817,9 @@
       <c r="C12" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="F12" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
@@ -5652,6 +5831,9 @@
       <c r="C13" s="9" t="s">
         <v>75</v>
       </c>
+      <c r="F13" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
@@ -5663,6 +5845,9 @@
       <c r="C14" s="9" t="s">
         <v>105</v>
       </c>
+      <c r="F14" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
@@ -5674,6 +5859,9 @@
       <c r="C15" s="9" t="s">
         <v>106</v>
       </c>
+      <c r="F15" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
@@ -5685,8 +5873,11 @@
       <c r="C16" s="9" t="s">
         <v>107</v>
       </c>
+      <c r="F16" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
@@ -5696,8 +5887,11 @@
       <c r="C17" s="9" t="s">
         <v>101</v>
       </c>
+      <c r="F17" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>108</v>
       </c>
@@ -5707,8 +5901,11 @@
       <c r="C18" s="9" t="s">
         <v>124</v>
       </c>
+      <c r="F18" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>109</v>
       </c>
@@ -5718,8 +5915,11 @@
       <c r="C19" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="F19" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>110</v>
       </c>
@@ -5729,8 +5929,11 @@
       <c r="C20" s="9" t="s">
         <v>126</v>
       </c>
+      <c r="F20" t="s">
+        <v>203</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>111</v>
       </c>
@@ -5740,8 +5943,11 @@
       <c r="C21" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="F21" t="s">
+        <v>204</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>112</v>
       </c>
@@ -5751,8 +5957,11 @@
       <c r="C22" s="9" t="s">
         <v>128</v>
       </c>
+      <c r="F22" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>113</v>
       </c>
@@ -5762,8 +5971,11 @@
       <c r="C23" s="9" t="s">
         <v>129</v>
       </c>
+      <c r="F23" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>114</v>
       </c>
@@ -5773,8 +5985,11 @@
       <c r="C24" s="9" t="s">
         <v>130</v>
       </c>
+      <c r="F24" t="s">
+        <v>207</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>115</v>
       </c>
@@ -5784,8 +5999,11 @@
       <c r="C25" s="9" t="s">
         <v>131</v>
       </c>
+      <c r="F25" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>116</v>
       </c>
@@ -5795,8 +6013,11 @@
       <c r="C26" s="9" t="s">
         <v>132</v>
       </c>
+      <c r="F26" t="s">
+        <v>209</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>117</v>
       </c>
@@ -5806,8 +6027,11 @@
       <c r="C27" s="9" t="s">
         <v>133</v>
       </c>
+      <c r="F27" t="s">
+        <v>210</v>
+      </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>118</v>
       </c>
@@ -5817,8 +6041,11 @@
       <c r="C28" s="9" t="s">
         <v>134</v>
       </c>
+      <c r="F28" t="s">
+        <v>211</v>
+      </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>119</v>
       </c>
@@ -5828,8 +6055,11 @@
       <c r="C29" s="9" t="s">
         <v>135</v>
       </c>
+      <c r="F29" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>120</v>
       </c>
@@ -5839,8 +6069,11 @@
       <c r="C30" s="9" t="s">
         <v>136</v>
       </c>
+      <c r="F30" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>121</v>
       </c>
@@ -5850,8 +6083,11 @@
       <c r="C31" s="9" t="s">
         <v>137</v>
       </c>
+      <c r="F31" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>122</v>
       </c>
@@ -5861,8 +6097,11 @@
       <c r="C32" s="9" t="s">
         <v>138</v>
       </c>
+      <c r="F32" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>123</v>
       </c>
@@ -5872,8 +6111,11 @@
       <c r="C33" s="9" t="s">
         <v>139</v>
       </c>
+      <c r="F33" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>140</v>
       </c>
@@ -5883,8 +6125,11 @@
       <c r="C34" s="9" t="s">
         <v>144</v>
       </c>
+      <c r="F34" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>141</v>
       </c>
@@ -5894,8 +6139,11 @@
       <c r="C35" s="9" t="s">
         <v>145</v>
       </c>
+      <c r="F35" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>142</v>
       </c>
@@ -5905,8 +6153,11 @@
       <c r="C36" s="9" t="s">
         <v>146</v>
       </c>
+      <c r="F36" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>143</v>
       </c>
@@ -5916,8 +6167,11 @@
       <c r="C37" s="9" t="s">
         <v>147</v>
       </c>
+      <c r="F37" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>148</v>
       </c>
@@ -5927,8 +6181,11 @@
       <c r="C38" s="9" t="s">
         <v>159</v>
       </c>
+      <c r="F38" t="s">
+        <v>221</v>
+      </c>
     </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>149</v>
       </c>
@@ -5938,8 +6195,11 @@
       <c r="C39" s="9" t="s">
         <v>160</v>
       </c>
+      <c r="F39" t="s">
+        <v>222</v>
+      </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>150</v>
       </c>
@@ -5949,8 +6209,11 @@
       <c r="C40" s="9" t="s">
         <v>161</v>
       </c>
+      <c r="F40" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>151</v>
       </c>
@@ -5960,8 +6223,11 @@
       <c r="C41" s="9" t="s">
         <v>162</v>
       </c>
+      <c r="F41" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>152</v>
       </c>
@@ -5971,8 +6237,11 @@
       <c r="C42" s="9" t="s">
         <v>163</v>
       </c>
+      <c r="F42" t="s">
+        <v>225</v>
+      </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>153</v>
       </c>
@@ -5982,8 +6251,11 @@
       <c r="C43" s="9" t="s">
         <v>164</v>
       </c>
+      <c r="F43" t="s">
+        <v>226</v>
+      </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>154</v>
       </c>
@@ -5993,8 +6265,11 @@
       <c r="C44" s="9" t="s">
         <v>165</v>
       </c>
+      <c r="F44" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -6004,8 +6279,11 @@
       <c r="C45" s="9" t="s">
         <v>166</v>
       </c>
+      <c r="F45" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>156</v>
       </c>
@@ -6015,8 +6293,11 @@
       <c r="C46" s="9" t="s">
         <v>167</v>
       </c>
+      <c r="F46" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>157</v>
       </c>
@@ -6026,8 +6307,11 @@
       <c r="C47" s="9" t="s">
         <v>168</v>
       </c>
+      <c r="F47" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>158</v>
       </c>
@@ -6037,8 +6321,11 @@
       <c r="C48" s="9" t="s">
         <v>169</v>
       </c>
+      <c r="F48" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>170</v>
       </c>
@@ -6048,8 +6335,11 @@
       <c r="C49" s="9" t="s">
         <v>172</v>
       </c>
+      <c r="F49" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>171</v>
       </c>
@@ -6059,8 +6349,11 @@
       <c r="C50" s="9" t="s">
         <v>173</v>
       </c>
+      <c r="F50" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>174</v>
       </c>
@@ -6070,8 +6363,11 @@
       <c r="C51" s="9" t="s">
         <v>176</v>
       </c>
+      <c r="F51" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>175</v>
       </c>
@@ -6081,19 +6377,22 @@
       <c r="C52" s="9" t="s">
         <v>177</v>
       </c>
+      <c r="F52" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add 2015-2016 deployment info
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE350561-0D83-0846-86B0-B6F9E617AFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3BFD8-BC79-2041-9DD3-30791A75D78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Detectors" sheetId="8" r:id="rId8"/>
     <sheet name="SensingPerspective" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="253">
   <si>
     <t>Attribute</t>
   </si>
@@ -260,18 +260,9 @@
     <t>nhanes-kb:INS-INQ_Family_J-QUESTIONNAIRE</t>
   </si>
   <si>
-    <t>Family Questionnaire - Income</t>
-  </si>
-  <si>
-    <t>Family Questionnaire - Demographic Background</t>
-  </si>
-  <si>
     <t>nhanes-kb:INS-DMQ_J-QUESTIONNAIRE</t>
   </si>
   <si>
-    <t>Sample Person Questionnaire - Demographic</t>
-  </si>
-  <si>
     <t>nhanes-kb:INS-DSQ_J-QUESTIONNAIRE</t>
   </si>
   <si>
@@ -347,9 +338,6 @@
     <t>Sample Person Questionnaire - Cardiovascular Disease</t>
   </si>
   <si>
-    <t>Sample Person Questionnaire - Dietary Supplements and Prescription Medication</t>
-  </si>
-  <si>
     <t>nhanes-kb:INS-DEQ_J-QUESTIONNAIRE</t>
   </si>
   <si>
@@ -753,6 +741,66 @@
   </si>
   <si>
     <t>skos:definition</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_Family_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Demographic Background (2017-2018)</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Demographic Background (2015-2016)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/DMQ_Family_I.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-INQ_Family_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Income (2017-2018)</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Income (2015-2016)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/INQ_Family_I.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Demographic (2017-2018)</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Demographic (2015-2016)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/DMQ_I.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DSQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Dietary Supplements and Prescription Medication (2017-2018)</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Dietary Supplements and Prescription Medication (2015-2016)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/DSQ_I.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_Family_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-INQ_Family_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DSQ_I-QUESTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -2260,15 +2308,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="33.5" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
@@ -2302,39 +2350,39 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>70</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>80</v>
+      <c r="A3" s="8" t="s">
+        <v>249</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>28</v>
@@ -2342,19 +2390,19 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>28</v>
@@ -2362,21 +2410,101 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>82</v>
+        <v>250</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5563,17 +5691,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="58.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
-    <col min="3" max="3" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="75.1640625" bestFit="1" customWidth="1"/>
@@ -5595,26 +5723,26 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5642,15 +5770,15 @@
         <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>234</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -5673,718 +5801,792 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>189</v>
-      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>91</v>
+        <v>238</v>
       </c>
       <c r="F7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>90</v>
+        <v>237</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>92</v>
+        <v>239</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>106</v>
+        <v>242</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>107</v>
+        <v>243</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="F20" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>111</v>
+        <v>245</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="F21" t="s">
-        <v>204</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F23" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F26" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F29" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F30" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F31" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F32" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F34" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F36" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F38" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F40" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="F41" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F42" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F43" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F44" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F45" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F46" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F47" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F48" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F49" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F50" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F52" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F56" t="s">
+        <v>231</v>
+      </c>
+    </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7328,6 +7530,10 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add 2013-2014 instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3BFD8-BC79-2041-9DD3-30791A75D78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE8047-0A74-504C-91DB-511526F53845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="269">
   <si>
     <t>Attribute</t>
   </si>
@@ -801,6 +801,54 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-DSQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_Family_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Demographic Background (2013-2014)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/DMQ_Family_H.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-INQ_Family_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Income (2013-2014)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/INQ_Family_H.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Demographic (2013-2014)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/DMQ_H.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DSQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Dietary Supplements and Prescription Medication (2013-2014)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/DSQ_H.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_Family_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-INQ_Family_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DSQ_H-QUESTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -2308,10 +2356,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,8 +2437,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>77</v>
+      <c r="A4" s="8" t="s">
+        <v>265</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -2398,8 +2446,8 @@
       <c r="C4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>71</v>
+      <c r="D4" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>76</v>
@@ -2410,7 +2458,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>250</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
@@ -2419,7 +2467,7 @@
         <v>75</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>76</v>
@@ -2430,7 +2478,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>78</v>
+        <v>250</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -2439,7 +2487,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>72</v>
+        <v>237</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>76</v>
@@ -2450,7 +2498,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -2459,7 +2507,7 @@
         <v>75</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>76</v>
@@ -2470,7 +2518,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
@@ -2479,7 +2527,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>76</v>
@@ -2490,7 +2538,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -2499,12 +2547,92 @@
         <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5691,10 +5819,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5837,760 +5965,834 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>82</v>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>183</v>
-      </c>
+      <c r="C5" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F7" t="s">
-        <v>185</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F8" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>88</v>
+        <v>239</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>87</v>
+        <v>256</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>242</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>241</v>
+        <v>93</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>243</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="F17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>99</v>
+        <v>241</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="F18" t="s">
-        <v>194</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>103</v>
+        <v>260</v>
       </c>
       <c r="F19" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>246</v>
+        <v>101</v>
       </c>
       <c r="F20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>245</v>
+        <v>99</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>247</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>248</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>121</v>
+        <v>246</v>
       </c>
       <c r="F23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>122</v>
+        <v>247</v>
       </c>
       <c r="F24" t="s">
-        <v>199</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>123</v>
+        <v>263</v>
       </c>
       <c r="F25" t="s">
-        <v>200</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F27" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F30" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F33" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F36" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F38" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F39" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F41" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F42" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F43" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F47" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F48" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F49" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F50" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F51" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F52" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F54" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F55" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F56" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F57" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F59" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F60" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7534,6 +7736,10 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
`HIQ` instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE8047-0A74-504C-91DB-511526F53845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4186C0D0-C082-9644-827E-3A479A87E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="278">
   <si>
     <t>Attribute</t>
   </si>
@@ -410,9 +410,6 @@
     <t>Sample Person Questionnaire - Early Childhood</t>
   </si>
   <si>
-    <t>Sample Person Questionnaire - Health Insurance</t>
-  </si>
-  <si>
     <t>Sample Person Questionnaire - Hepatitis</t>
   </si>
   <si>
@@ -849,6 +846,36 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-DSQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-HIQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Health Insurance (2017-2018)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-HIQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-HIQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Health Insurance (2015-2016)</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Health Insurance (2013-2014)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/HIQ_I.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/HIQ_H.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-HIQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-HIQ_H-QUESTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -2356,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2418,7 +2445,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
@@ -2427,7 +2454,7 @@
         <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>76</v>
@@ -2438,7 +2465,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -2447,7 +2474,7 @@
         <v>75</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>76</v>
@@ -2478,7 +2505,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -2487,7 +2514,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>76</v>
@@ -2498,7 +2525,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -2507,7 +2534,7 @@
         <v>75</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>76</v>
@@ -2538,7 +2565,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -2547,7 +2574,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>76</v>
@@ -2558,7 +2585,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -2567,7 +2594,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>76</v>
@@ -2598,7 +2625,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>25</v>
@@ -2607,7 +2634,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>76</v>
@@ -2618,7 +2645,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -2627,12 +2654,72 @@
         <v>75</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5819,10 +5906,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5851,10 +5938,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -5862,7 +5949,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>81</v>
@@ -5870,7 +5957,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5898,15 +5985,15 @@
         <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -5931,18 +6018,18 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -5967,18 +6054,18 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>254</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -6006,13 +6093,13 @@
         <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>83</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -6020,7 +6107,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>85</v>
@@ -6028,7 +6115,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -6056,41 +6143,41 @@
         <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" t="s">
         <v>239</v>
-      </c>
-      <c r="F9" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="F10" t="s">
         <v>257</v>
-      </c>
-      <c r="F10" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,13 +6185,13 @@
         <v>86</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6112,13 +6199,13 @@
         <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6126,13 +6213,13 @@
         <v>90</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6140,13 +6227,13 @@
         <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6154,13 +6241,13 @@
         <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6168,13 +6255,13 @@
         <v>93</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6182,41 +6269,41 @@
         <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18" t="s">
         <v>243</v>
-      </c>
-      <c r="F18" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="F19" t="s">
         <v>260</v>
-      </c>
-      <c r="F19" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6224,13 +6311,13 @@
         <v>98</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>101</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6238,13 +6325,13 @@
         <v>99</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6252,13 +6339,13 @@
         <v>100</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6266,41 +6353,41 @@
         <v>73</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F24" t="s">
         <v>247</v>
-      </c>
-      <c r="F24" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="F25" t="s">
         <v>263</v>
-      </c>
-      <c r="F25" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6308,13 +6395,13 @@
         <v>104</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6322,13 +6409,13 @@
         <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>121</v>
       </c>
       <c r="F27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6336,465 +6423,491 @@
         <v>106</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>122</v>
+        <v>269</v>
       </c>
       <c r="F28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>107</v>
+        <v>270</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" t="s">
-        <v>200</v>
+        <v>272</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>124</v>
+        <v>273</v>
       </c>
       <c r="F30" t="s">
-        <v>201</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F32" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F33" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F34" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F35" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F40" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F42" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F43" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F44" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F45" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F47" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F48" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F49" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F50" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F51" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F52" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F53" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F54" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F55" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F56" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F57" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F58" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F60" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="F60" t="s">
-        <v>231</v>
+      <c r="F61" t="s">
+        <v>229</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F62" t="s">
+        <v>230</v>
+      </c>
+    </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7740,6 +7853,8 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
2009-2010 instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4186C0D0-C082-9644-827E-3A479A87E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758FCCAD-78FD-6F4C-92CE-A8E72D7969E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="298">
   <si>
     <t>Attribute</t>
   </si>
@@ -876,6 +876,66 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-HIQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_Family_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Demographic Background (2009-2010)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-INQ_Family_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Family Questionnaire - Income (2009-2010)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DMQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Demographic (2009-2010)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-DSQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Dietary Supplements and Prescription Medication (2009-2010)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-HIQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Health Insurance (2009-2010)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/dmq_f_eng.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/inq_f_eng.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/dmq_f.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/dsq_f.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/hiq_f.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_Family_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-INQ_Family_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DSQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-HIQ_F-QUESTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -2383,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,8 +2544,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>77</v>
+      <c r="A5" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
@@ -2493,8 +2553,8 @@
       <c r="C5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>71</v>
+      <c r="D5" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>76</v>
@@ -2505,7 +2565,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
@@ -2514,7 +2574,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>236</v>
+        <v>71</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>76</v>
@@ -2525,7 +2585,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -2534,7 +2594,7 @@
         <v>75</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>76</v>
@@ -2545,7 +2605,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>78</v>
+        <v>265</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
@@ -2554,7 +2614,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>72</v>
+        <v>255</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>76</v>
@@ -2565,7 +2625,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>250</v>
+        <v>294</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -2574,7 +2634,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>76</v>
@@ -2585,7 +2645,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>266</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -2594,7 +2654,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>258</v>
+        <v>72</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>76</v>
@@ -2605,7 +2665,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>79</v>
+        <v>250</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -2614,7 +2674,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>73</v>
+        <v>240</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>76</v>
@@ -2625,7 +2685,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>25</v>
@@ -2634,7 +2694,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>76</v>
@@ -2645,7 +2705,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -2654,7 +2714,7 @@
         <v>75</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>76</v>
@@ -2665,7 +2725,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>268</v>
+        <v>79</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -2674,7 +2734,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>76</v>
@@ -2685,7 +2745,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
@@ -2694,7 +2754,7 @@
         <v>75</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>76</v>
@@ -2705,7 +2765,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>25</v>
@@ -2714,12 +2774,112 @@
         <v>75</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5906,10 +6066,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z1009"/>
+  <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="C36" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6088,844 +6248,931 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>82</v>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
-        <v>182</v>
-      </c>
+      <c r="C6" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>182</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="F8" t="s">
-        <v>184</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>236</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F9" t="s">
-        <v>239</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>88</v>
+        <v>256</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>87</v>
+        <v>280</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>89</v>
+        <v>281</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>241</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>240</v>
+        <v>93</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>242</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>258</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="F19" t="s">
-        <v>260</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>98</v>
+        <v>240</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="F20" t="s">
-        <v>192</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>99</v>
+        <v>258</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>102</v>
+        <v>259</v>
       </c>
       <c r="F21" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>100</v>
+        <v>282</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>103</v>
+        <v>283</v>
       </c>
       <c r="F22" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>245</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>244</v>
+        <v>99</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>246</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>261</v>
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>263</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>120</v>
+        <v>245</v>
       </c>
       <c r="F26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>105</v>
+        <v>244</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>121</v>
+        <v>246</v>
       </c>
       <c r="F27" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>106</v>
+        <v>261</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F28" t="s">
-        <v>198</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>274</v>
+        <v>285</v>
+      </c>
+      <c r="F29" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>271</v>
+        <v>104</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>273</v>
+        <v>120</v>
       </c>
       <c r="F30" t="s">
-        <v>275</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>123</v>
+        <v>269</v>
       </c>
       <c r="F32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>109</v>
+        <v>270</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" t="s">
-        <v>201</v>
+        <v>272</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>125</v>
+        <v>273</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>111</v>
+        <v>286</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>126</v>
+        <v>287</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F36" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F39" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F40" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F42" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F43" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F44" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F45" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F46" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="F48" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="F51" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="F52" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F54" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F55" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F56" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F57" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F58" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F59" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F60" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F61" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F62" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F63" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F64" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F66" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F67" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7855,6 +8102,11 @@
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
lab results instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758FCCAD-78FD-6F4C-92CE-A8E72D7969E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6305BF84-7A75-CA44-B3C7-4067233689BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="314">
   <si>
     <t>Attribute</t>
   </si>
@@ -936,6 +936,54 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-HIQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Roche/Hitachi Cobas 6000 Analyzer</t>
+  </si>
+  <si>
+    <t>Roche Diagnostics</t>
+  </si>
+  <si>
+    <t>nhanes-kb:ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
+  </si>
+  <si>
+    <t>Generic Roche/Hitachi Cobas 6000 Analyzer</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:PLT-GENERIC-PLATFORM</t>
+  </si>
+  <si>
+    <t>nhanes-kb:MOLECULAR-WORK-AREA</t>
+  </si>
+  <si>
+    <t>vstoi:OpticalInstrument</t>
+  </si>
+  <si>
+    <t>Molecular Work Area</t>
+  </si>
+  <si>
+    <t>vstoi:PhysicalInstrument</t>
+  </si>
+  <si>
+    <t>nhanes-kb:ROCHE-HITACHI-COBAS-C-ANALYZER-C311</t>
+  </si>
+  <si>
+    <t>Roche/Hitachi Cobas C Analyzer – C311</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-ROCHE-HITACHI-COBAS-C-ANALYZER-C311</t>
+  </si>
+  <si>
+    <t>Generic Roche/Hitachi Cobas C Analyzer C311</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-C-ANALYZER-C311</t>
   </si>
 </sst>
 </file>
@@ -2443,18 +2491,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="50.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="33.5" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.33203125" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
@@ -2880,6 +2928,46 @@
         <v>76</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D22" t="s">
+        <v>301</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3932,10 +4020,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N990"/>
+  <dimension ref="A1:N989"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4024,6 +4112,7 @@
         <v>50</v>
       </c>
     </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5003,7 +5092,6 @@
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5012,17 +5100,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M997"/>
+  <dimension ref="A1:M998"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
@@ -5078,7 +5166,45 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" t="s">
+        <v>307</v>
+      </c>
+    </row>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6058,6 +6184,7 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6068,14 +6195,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="C36" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A47" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="1" max="1" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -7160,8 +7287,28 @@
         <v>230</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>301</v>
+      </c>
+      <c r="B68" t="s">
+        <v>300</v>
+      </c>
+      <c r="C68" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GHB instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DFE28E-2E12-1840-B0BB-2C480F93F024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4821D1-C36C-974F-BA83-D3C7048B419B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="327">
   <si>
     <t>Attribute</t>
   </si>
@@ -987,6 +987,42 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-DIQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:TOSOH-G8-GLYCOHEMOGLOBIN-ANALYZER</t>
+  </si>
+  <si>
+    <t>Tosoh G8 Glycohemoglobin Analyzer</t>
+  </si>
+  <si>
+    <t>Tosoh Bioscience, Inc.</t>
+  </si>
+  <si>
+    <t>nhanes-kb:TRINITY-BIOTECH-PREMIER-HB9210-AUTOMATED-HPLC-SYSTEM</t>
+  </si>
+  <si>
+    <t>Trinity Biotech Premier Hb9210 Automated HPLC System</t>
+  </si>
+  <si>
+    <t>Trinity Biotech</t>
+  </si>
+  <si>
+    <t>Generic Tosoh G8 Glycohemoglobin Analyzer</t>
+  </si>
+  <si>
+    <t>Generic Trinity Biotech Premier Hb9210 Automated HPLC System</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-TOSOH-G8-GLYCOHEMOGLOBIN-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-TRINITY-BIOTECH-PREMIER-HB9210-AUTOMATED-HPLC-SYSTEM</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-TOSOH-G8-GLYCOHEMOGLOBIN-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-TRINITY-BIOTECH-PREMIER-HB9210-AUTOMATED-HPLC-SYSTEM</t>
   </si>
 </sst>
 </file>
@@ -2494,18 +2530,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="33.5" customWidth="1"/>
-    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.33203125" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
@@ -2991,6 +3027,46 @@
         <v>76</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5126,14 +5202,14 @@
   <dimension ref="A1:M998"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
@@ -5226,6 +5302,34 @@
       </c>
       <c r="C4" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6218,14 +6322,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A59" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -7332,8 +7436,28 @@
         <v>312</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
additional instruments for lab results
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2C081D-DCBF-424F-B76F-D1F67948E769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8865B8C2-5862-AC4B-B985-0F79EB878B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23100" yWindow="-21520" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="361">
   <si>
     <t>Attribute</t>
   </si>
@@ -1092,6 +1092,39 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-BECKMAN-COULTER-UNICEL-DXC-660i-SYNCHRON</t>
+  </si>
+  <si>
+    <t>nhanes-kb:ROCHE-MODULAR-P-CHEMISTRY-ANALYZER</t>
+  </si>
+  <si>
+    <t>Roche Modular P Chemistry Analyzer</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-ROCHE-MODULAR-P-CHEMISTRY-ANALYZER</t>
+  </si>
+  <si>
+    <t>Generic Roche Modular P Chemistry Analyzer</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-ROCHE-MODULAR-P-CHEMISTRY-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:TOSOH-G7-AUTOMATED-HPLC-ANALYZER</t>
+  </si>
+  <si>
+    <t>Tosoh G7 Automated HPLC Analyzer</t>
+  </si>
+  <si>
+    <t>Tosoh Medics, Inc.</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-TOSOH-G7-AUTOMATED-HPLC-ANALYZER</t>
+  </si>
+  <si>
+    <t>Generic Tosoh G7 Automated HPLC Analyzer</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-TOSOH-G7-AUTOMATED-HPLC-ANALYZER</t>
   </si>
 </sst>
 </file>
@@ -2599,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3159,9 +3192,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>25</v>
@@ -3170,7 +3203,7 @@
         <v>303</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>322</v>
+        <v>352</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>76</v>
@@ -3179,9 +3212,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>325</v>
+        <v>360</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>25</v>
@@ -3190,7 +3223,7 @@
         <v>303</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>323</v>
+        <v>358</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>76</v>
@@ -3201,7 +3234,7 @@
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>25</v>
@@ -3210,7 +3243,7 @@
         <v>303</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>76</v>
@@ -3221,7 +3254,7 @@
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>25</v>
@@ -3230,12 +3263,52 @@
         <v>303</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5368,10 +5441,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M998"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5463,74 +5536,100 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>304</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>305</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>317</v>
+        <v>355</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>307</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>319</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>307</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="D7" t="s">
-        <v>343</v>
+        <v>315</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>307</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6509,6 +6608,8 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6517,10 +6618,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z1017"/>
+  <dimension ref="A1:Z1019"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A76" sqref="A75:A76"/>
+    <sheetView topLeftCell="A63" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7677,50 +7778,70 @@
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
-        <v>322</v>
+        <v>352</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>314</v>
+        <v>350</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>320</v>
+        <v>353</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
-        <v>323</v>
+        <v>358</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>317</v>
+        <v>355</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>321</v>
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8660,6 +8781,8 @@
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
pregnancy tests instruments and deployments
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8865B8C2-5862-AC4B-B985-0F79EB878B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155F8F3B-C5C3-AB40-8948-B8E9B7C763A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23100" yWindow="-21520" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="366">
   <si>
     <t>Attribute</t>
   </si>
@@ -1125,6 +1125,21 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-TOSOH-G7-AUTOMATED-HPLC-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:BECKMAN-COULTER-ICON-25-HCG-URINE-SERUM-TEST-KIT</t>
+  </si>
+  <si>
+    <t>Beckman Coulter ICON 25 hCG Test</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-BECKMAN-COULTER-ICON-25-HCG-URINE-SERUM-TEST-KIT</t>
+  </si>
+  <si>
+    <t>Generic Beckman Coulter ICON 25 hCG Test</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BECKMAN-COULTER-ICON-25-HCG-URINE-SERUM-TEST-KIT</t>
   </si>
 </sst>
 </file>
@@ -2632,10 +2647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3309,6 +3324,26 @@
         <v>76</v>
       </c>
       <c r="F33" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5444,7 +5479,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5627,6 +5662,20 @@
         <v>342</v>
       </c>
       <c r="D10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D11" t="s">
         <v>343</v>
       </c>
     </row>
@@ -6621,7 +6670,7 @@
   <dimension ref="A1:Z1019"/>
   <sheetViews>
     <sheetView topLeftCell="A63" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7842,7 +7891,17 @@
         <v>347</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
`BPQ` deployments and DAs
</commit_message>
<xml_diff>
--- a/metadata/DPL-NHANES.xlsx
+++ b/metadata/DPL-NHANES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155F8F3B-C5C3-AB40-8948-B8E9B7C763A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8DF8DD-10A3-8841-A0B9-1F0106966688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23100" yWindow="-21520" windowWidth="28800" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23100" yWindow="-21520" windowWidth="38680" windowHeight="15660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="379">
   <si>
     <t>Attribute</t>
   </si>
@@ -332,9 +332,6 @@
     <t>Sample Person Questionnaire - Audiometry</t>
   </si>
   <si>
-    <t>Sample Person Questionnaire - Blood Pressure</t>
-  </si>
-  <si>
     <t>Sample Person Questionnaire - Cardiovascular Disease</t>
   </si>
   <si>
@@ -1140,6 +1137,48 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-BECKMAN-COULTER-ICON-25-HCG-URINE-SERUM-TEST-KIT</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Blood Pressure (2017-2018)</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-BPQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-BPQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:INS-BPQ_F-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Blood Pressure (2015-2016)</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Blood Pressure (2013-2014)</t>
+  </si>
+  <si>
+    <t>Sample Person Questionnaire - Blood Pressure (2009-2010)</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2015-2016/questionnaires/BPQ_I.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2013-2014/questionnaires/BPQ_H.pdf</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/data/nhanes/2009-2010/questionnaires/bpq_f.pdf</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BPQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BPQ_I-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BPQ_H-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BPQ_F-QUESTIONNAIRE</t>
   </si>
 </sst>
 </file>
@@ -2647,10 +2686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:F34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2709,7 +2748,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
@@ -2718,7 +2757,7 @@
         <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>76</v>
@@ -2729,7 +2768,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -2738,7 +2777,7 @@
         <v>75</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>76</v>
@@ -2749,7 +2788,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
@@ -2758,7 +2797,7 @@
         <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>76</v>
@@ -2789,7 +2828,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -2798,7 +2837,7 @@
         <v>75</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>76</v>
@@ -2809,7 +2848,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
@@ -2818,7 +2857,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>76</v>
@@ -2829,7 +2868,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -2838,7 +2877,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>76</v>
@@ -2849,7 +2888,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>313</v>
+        <v>375</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -2858,7 +2897,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>76</v>
@@ -2869,7 +2908,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -2878,7 +2917,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>76</v>
@@ -2889,7 +2928,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>25</v>
@@ -2898,7 +2937,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>76</v>
@@ -2909,7 +2948,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>338</v>
+        <v>378</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -2918,7 +2957,7 @@
         <v>75</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>76</v>
@@ -2929,7 +2968,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>78</v>
+        <v>312</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -2938,7 +2977,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>76</v>
@@ -2949,7 +2988,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>249</v>
+        <v>335</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
@@ -2958,7 +2997,7 @@
         <v>75</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>239</v>
+        <v>326</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>76</v>
@@ -2969,7 +3008,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>265</v>
+        <v>336</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>25</v>
@@ -2978,7 +3017,7 @@
         <v>75</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>257</v>
+        <v>327</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>76</v>
@@ -2989,7 +3028,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>294</v>
+        <v>337</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>25</v>
@@ -2998,7 +3037,7 @@
         <v>75</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>281</v>
+        <v>328</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>76</v>
@@ -3009,7 +3048,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>25</v>
@@ -3018,7 +3057,7 @@
         <v>75</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>76</v>
@@ -3029,7 +3068,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>25</v>
@@ -3038,7 +3077,7 @@
         <v>75</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>76</v>
@@ -3049,7 +3088,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>25</v>
@@ -3058,7 +3097,7 @@
         <v>75</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>76</v>
@@ -3069,7 +3108,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>25</v>
@@ -3078,7 +3117,7 @@
         <v>75</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>76</v>
@@ -3089,7 +3128,7 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>267</v>
+        <v>79</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>25</v>
@@ -3098,7 +3137,7 @@
         <v>75</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>76</v>
@@ -3109,7 +3148,7 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>25</v>
@@ -3118,7 +3157,7 @@
         <v>75</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>76</v>
@@ -3129,7 +3168,7 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>25</v>
@@ -3138,7 +3177,7 @@
         <v>75</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>76</v>
@@ -3149,7 +3188,7 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>25</v>
@@ -3158,7 +3197,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>76</v>
@@ -3169,16 +3208,16 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="D26" t="s">
-        <v>300</v>
+        <v>75</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>76</v>
@@ -3189,16 +3228,16 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>303</v>
+        <v>75</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>310</v>
+        <v>268</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>76</v>
@@ -3209,16 +3248,16 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>354</v>
+        <v>275</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>303</v>
+        <v>75</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>352</v>
+        <v>269</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>76</v>
@@ -3229,16 +3268,16 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>360</v>
+        <v>295</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>303</v>
+        <v>75</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>358</v>
+        <v>284</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>76</v>
@@ -3247,18 +3286,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>322</v>
+        <v>302</v>
+      </c>
+      <c r="D30" t="s">
+        <v>299</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>76</v>
@@ -3267,18 +3306,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>76</v>
@@ -3287,18 +3326,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>76</v>
@@ -3307,18 +3346,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>76</v>
@@ -3329,21 +3368,101 @@
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5544,139 +5663,139 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
         <v>297</v>
-      </c>
-      <c r="D2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>309</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>351</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" t="s">
         <v>304</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>305</v>
-      </c>
-      <c r="C5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>315</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>318</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" t="s">
         <v>342</v>
-      </c>
-      <c r="D10" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>362</v>
-      </c>
       <c r="D11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6667,10 +6786,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z1019"/>
+  <dimension ref="A1:Z1022"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6699,10 +6818,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -6710,7 +6829,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>81</v>
@@ -6718,7 +6837,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -6746,15 +6865,15 @@
         <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -6779,18 +6898,18 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -6815,18 +6934,18 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -6851,18 +6970,18 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>278</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -6890,13 +7009,13 @@
         <v>82</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -6904,7 +7023,7 @@
         <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>85</v>
@@ -6912,7 +7031,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6940,55 +7059,55 @@
         <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" t="s">
         <v>237</v>
-      </c>
-      <c r="F10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="F11" t="s">
         <v>255</v>
-      </c>
-      <c r="F11" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>280</v>
-      </c>
       <c r="F12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6996,13 +7115,13 @@
         <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7010,13 +7129,13 @@
         <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7024,13 +7143,13 @@
         <v>90</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7038,13 +7157,13 @@
         <v>91</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7052,873 +7171,912 @@
         <v>92</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>96</v>
+        <v>365</v>
       </c>
       <c r="F17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>93</v>
+        <v>366</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>97</v>
+        <v>369</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>72</v>
+        <v>367</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>240</v>
+        <v>370</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>239</v>
+        <v>368</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>241</v>
+        <v>371</v>
       </c>
       <c r="F20" t="s">
-        <v>242</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>257</v>
+        <v>93</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>258</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>259</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>281</v>
+        <v>72</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="F22" t="s">
-        <v>289</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>98</v>
+        <v>238</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="F23" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>99</v>
+        <v>256</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>326</v>
+        <v>257</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>327</v>
+        <v>280</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>330</v>
+        <v>281</v>
       </c>
       <c r="F25" t="s">
-        <v>333</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>328</v>
+        <v>97</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>331</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>334</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>329</v>
+        <v>98</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F27" t="s">
-        <v>335</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>100</v>
+        <v>326</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>102</v>
+        <v>329</v>
       </c>
       <c r="F28" t="s">
-        <v>193</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>73</v>
+        <v>327</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>244</v>
+        <v>330</v>
       </c>
       <c r="F29" t="s">
-        <v>194</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>243</v>
+        <v>328</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="F30" t="s">
-        <v>246</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>260</v>
+        <v>99</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>261</v>
+        <v>101</v>
       </c>
       <c r="F31" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>283</v>
+        <v>73</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="F32" t="s">
-        <v>290</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>119</v>
+        <v>244</v>
       </c>
       <c r="F33" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="F34" t="s">
-        <v>196</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>105</v>
+        <v>282</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="F35" t="s">
-        <v>197</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>269</v>
+        <v>102</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>273</v>
+        <v>118</v>
+      </c>
+      <c r="F36" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>270</v>
+        <v>103</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>272</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
-        <v>274</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>285</v>
+        <v>104</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="F38" t="s">
-        <v>291</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>106</v>
+        <v>268</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" t="s">
-        <v>198</v>
+        <v>270</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>122</v>
+        <v>271</v>
       </c>
       <c r="F40" t="s">
-        <v>199</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>108</v>
+        <v>284</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>123</v>
+        <v>285</v>
       </c>
       <c r="F41" t="s">
-        <v>200</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F43" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F45" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F46" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F47" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F48" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F49" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F50" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F52" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F53" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F54" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="F55" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F56" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="F57" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F58" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F59" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F60" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F61" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F62" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F63" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F64" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F65" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F66" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F67" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F68" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F69" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F70" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F70" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="F72" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F73" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>299</v>
+      </c>
+      <c r="B74" t="s">
+        <v>298</v>
+      </c>
+      <c r="C74" t="s">
         <v>300</v>
-      </c>
-      <c r="B71" t="s">
-        <v>299</v>
-      </c>
-      <c r="C71" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>317</v>
+        <v>349</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8842,6 +9000,9 @@
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>